<commit_message>
Verion 0.9 bug fixes
</commit_message>
<xml_diff>
--- a/EECIP/App_Docs/ProjectImportTemplate.xlsx
+++ b/EECIP/App_Docs/ProjectImportTemplate.xlsx
@@ -9,7 +9,7 @@
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="122211"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
@@ -67,12 +67,60 @@
         </r>
       </text>
     </comment>
+    <comment ref="W5" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Author:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Mark with Y (along with filling out Import ID or EECIP Project ID column) to delete from EECIP</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="X5" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Author:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+You can use this to track the unique identifier from the external source you are importing data from. </t>
+        </r>
+      </text>
+    </comment>
   </commentList>
 </comments>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="30">
   <si>
     <t>Project Name</t>
   </si>
@@ -150,6 +198,18 @@
   </si>
   <si>
     <t>Project Contact</t>
+  </si>
+  <si>
+    <t>Mark with Y to delete this record from EECIP</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>External Source ID</t>
+  </si>
+  <si>
+    <t>Delete Ind</t>
   </si>
 </sst>
 </file>
@@ -582,7 +642,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:V256"/>
+  <dimension ref="A1:X256"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A6" sqref="A6"/>
@@ -611,14 +671,16 @@
     <col min="19" max="19" width="18.140625" bestFit="1" customWidth="1"/>
     <col min="20" max="20" width="23.5703125" customWidth="1"/>
     <col min="21" max="22" width="16.140625" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="40.7109375" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="17.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:24" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A1" s="7" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="2" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A2" s="8" t="s">
         <v>19</v>
       </c>
@@ -628,8 +690,11 @@
       <c r="V2" s="6" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="3" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="W2" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="3" spans="1:24" x14ac:dyDescent="0.25">
       <c r="U3" s="6" t="s">
         <v>22</v>
       </c>
@@ -637,7 +702,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="5" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
         <v>1</v>
       </c>
@@ -704,10 +769,18 @@
       <c r="V5" s="2" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="6" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="W5" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="X5" s="2" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="6" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A6" s="1"/>
-      <c r="B6" s="1"/>
+      <c r="B6" s="1" t="s">
+        <v>27</v>
+      </c>
       <c r="C6" s="1"/>
       <c r="D6" s="1"/>
       <c r="E6" s="3"/>
@@ -728,8 +801,10 @@
       <c r="T6" s="3"/>
       <c r="U6" s="1"/>
       <c r="V6" s="1"/>
-    </row>
-    <row r="7" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="W6" s="1"/>
+      <c r="X6" s="1"/>
+    </row>
+    <row r="7" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A7" s="1"/>
       <c r="B7" s="1"/>
       <c r="C7" s="1"/>
@@ -752,8 +827,10 @@
       <c r="T7" s="1"/>
       <c r="U7" s="1"/>
       <c r="V7" s="1"/>
-    </row>
-    <row r="8" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="W7" s="1"/>
+      <c r="X7" s="1"/>
+    </row>
+    <row r="8" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A8" s="1"/>
       <c r="B8" s="1"/>
       <c r="C8" s="1"/>
@@ -776,8 +853,10 @@
       <c r="T8" s="1"/>
       <c r="U8" s="1"/>
       <c r="V8" s="1"/>
-    </row>
-    <row r="9" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="W8" s="1"/>
+      <c r="X8" s="1"/>
+    </row>
+    <row r="9" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A9" s="1"/>
       <c r="B9" s="1"/>
       <c r="C9" s="1"/>
@@ -800,8 +879,10 @@
       <c r="T9" s="1"/>
       <c r="U9" s="1"/>
       <c r="V9" s="1"/>
-    </row>
-    <row r="10" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="W9" s="1"/>
+      <c r="X9" s="1"/>
+    </row>
+    <row r="10" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A10" s="1"/>
       <c r="B10" s="1"/>
       <c r="C10" s="1"/>
@@ -824,8 +905,10 @@
       <c r="T10" s="1"/>
       <c r="U10" s="1"/>
       <c r="V10" s="1"/>
-    </row>
-    <row r="11" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="W10" s="1"/>
+      <c r="X10" s="1"/>
+    </row>
+    <row r="11" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A11" s="1"/>
       <c r="B11" s="1"/>
       <c r="C11" s="1"/>
@@ -848,8 +931,10 @@
       <c r="T11" s="1"/>
       <c r="U11" s="1"/>
       <c r="V11" s="1"/>
-    </row>
-    <row r="12" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="W11" s="1"/>
+      <c r="X11" s="1"/>
+    </row>
+    <row r="12" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A12" s="1"/>
       <c r="B12" s="1"/>
       <c r="C12" s="1"/>
@@ -872,8 +957,10 @@
       <c r="T12" s="1"/>
       <c r="U12" s="1"/>
       <c r="V12" s="1"/>
-    </row>
-    <row r="13" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="W12" s="1"/>
+      <c r="X12" s="1"/>
+    </row>
+    <row r="13" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A13" s="1"/>
       <c r="B13" s="1"/>
       <c r="C13" s="1"/>
@@ -896,8 +983,10 @@
       <c r="T13" s="1"/>
       <c r="U13" s="1"/>
       <c r="V13" s="1"/>
-    </row>
-    <row r="14" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="W13" s="1"/>
+      <c r="X13" s="1"/>
+    </row>
+    <row r="14" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A14" s="1"/>
       <c r="B14" s="1"/>
       <c r="C14" s="1"/>
@@ -920,8 +1009,10 @@
       <c r="T14" s="1"/>
       <c r="U14" s="1"/>
       <c r="V14" s="1"/>
-    </row>
-    <row r="15" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="W14" s="1"/>
+      <c r="X14" s="1"/>
+    </row>
+    <row r="15" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A15" s="1"/>
       <c r="B15" s="1"/>
       <c r="C15" s="1"/>
@@ -944,8 +1035,10 @@
       <c r="T15" s="1"/>
       <c r="U15" s="1"/>
       <c r="V15" s="1"/>
-    </row>
-    <row r="16" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="W15" s="1"/>
+      <c r="X15" s="1"/>
+    </row>
+    <row r="16" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A16" s="1"/>
       <c r="B16" s="1"/>
       <c r="C16" s="1"/>
@@ -968,8 +1061,10 @@
       <c r="T16" s="1"/>
       <c r="U16" s="1"/>
       <c r="V16" s="1"/>
-    </row>
-    <row r="17" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="W16" s="1"/>
+      <c r="X16" s="1"/>
+    </row>
+    <row r="17" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A17" s="1"/>
       <c r="B17" s="1"/>
       <c r="C17" s="1"/>
@@ -992,8 +1087,10 @@
       <c r="T17" s="1"/>
       <c r="U17" s="1"/>
       <c r="V17" s="1"/>
-    </row>
-    <row r="18" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="W17" s="1"/>
+      <c r="X17" s="1"/>
+    </row>
+    <row r="18" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A18" s="1"/>
       <c r="B18" s="1"/>
       <c r="C18" s="1"/>
@@ -1016,8 +1113,10 @@
       <c r="T18" s="1"/>
       <c r="U18" s="1"/>
       <c r="V18" s="1"/>
-    </row>
-    <row r="19" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="W18" s="1"/>
+      <c r="X18" s="1"/>
+    </row>
+    <row r="19" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A19" s="1"/>
       <c r="B19" s="1"/>
       <c r="C19" s="1"/>
@@ -1040,8 +1139,10 @@
       <c r="T19" s="1"/>
       <c r="U19" s="1"/>
       <c r="V19" s="1"/>
-    </row>
-    <row r="20" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="W19" s="1"/>
+      <c r="X19" s="1"/>
+    </row>
+    <row r="20" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A20" s="1"/>
       <c r="B20" s="1"/>
       <c r="C20" s="1"/>
@@ -1064,8 +1165,10 @@
       <c r="T20" s="1"/>
       <c r="U20" s="1"/>
       <c r="V20" s="1"/>
-    </row>
-    <row r="21" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="W20" s="1"/>
+      <c r="X20" s="1"/>
+    </row>
+    <row r="21" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A21" s="1"/>
       <c r="B21" s="1"/>
       <c r="C21" s="1"/>
@@ -1088,8 +1191,10 @@
       <c r="T21" s="1"/>
       <c r="U21" s="1"/>
       <c r="V21" s="1"/>
-    </row>
-    <row r="22" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="W21" s="1"/>
+      <c r="X21" s="1"/>
+    </row>
+    <row r="22" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A22" s="1"/>
       <c r="B22" s="1"/>
       <c r="C22" s="1"/>
@@ -1112,8 +1217,10 @@
       <c r="T22" s="1"/>
       <c r="U22" s="1"/>
       <c r="V22" s="1"/>
-    </row>
-    <row r="23" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="W22" s="1"/>
+      <c r="X22" s="1"/>
+    </row>
+    <row r="23" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A23" s="1"/>
       <c r="B23" s="1"/>
       <c r="C23" s="1"/>
@@ -1136,8 +1243,10 @@
       <c r="T23" s="1"/>
       <c r="U23" s="1"/>
       <c r="V23" s="1"/>
-    </row>
-    <row r="24" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="W23" s="1"/>
+      <c r="X23" s="1"/>
+    </row>
+    <row r="24" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A24" s="1"/>
       <c r="B24" s="1"/>
       <c r="C24" s="1"/>
@@ -1160,8 +1269,10 @@
       <c r="T24" s="1"/>
       <c r="U24" s="1"/>
       <c r="V24" s="1"/>
-    </row>
-    <row r="25" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="W24" s="1"/>
+      <c r="X24" s="1"/>
+    </row>
+    <row r="25" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A25" s="1"/>
       <c r="B25" s="1"/>
       <c r="C25" s="1"/>
@@ -1184,8 +1295,10 @@
       <c r="T25" s="1"/>
       <c r="U25" s="1"/>
       <c r="V25" s="1"/>
-    </row>
-    <row r="26" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="W25" s="1"/>
+      <c r="X25" s="1"/>
+    </row>
+    <row r="26" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A26" s="1"/>
       <c r="B26" s="1"/>
       <c r="C26" s="1"/>
@@ -1208,8 +1321,10 @@
       <c r="T26" s="1"/>
       <c r="U26" s="1"/>
       <c r="V26" s="1"/>
-    </row>
-    <row r="27" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="W26" s="1"/>
+      <c r="X26" s="1"/>
+    </row>
+    <row r="27" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A27" s="1"/>
       <c r="B27" s="1"/>
       <c r="C27" s="1"/>
@@ -1232,8 +1347,10 @@
       <c r="T27" s="1"/>
       <c r="U27" s="1"/>
       <c r="V27" s="1"/>
-    </row>
-    <row r="28" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="W27" s="1"/>
+      <c r="X27" s="1"/>
+    </row>
+    <row r="28" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A28" s="1"/>
       <c r="B28" s="1"/>
       <c r="C28" s="1"/>
@@ -1256,8 +1373,10 @@
       <c r="T28" s="1"/>
       <c r="U28" s="1"/>
       <c r="V28" s="1"/>
-    </row>
-    <row r="29" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="W28" s="1"/>
+      <c r="X28" s="1"/>
+    </row>
+    <row r="29" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A29" s="1"/>
       <c r="B29" s="1"/>
       <c r="C29" s="1"/>
@@ -1280,8 +1399,10 @@
       <c r="T29" s="1"/>
       <c r="U29" s="1"/>
       <c r="V29" s="1"/>
-    </row>
-    <row r="30" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="W29" s="1"/>
+      <c r="X29" s="1"/>
+    </row>
+    <row r="30" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A30" s="1"/>
       <c r="B30" s="1"/>
       <c r="C30" s="1"/>
@@ -1304,8 +1425,10 @@
       <c r="T30" s="1"/>
       <c r="U30" s="1"/>
       <c r="V30" s="1"/>
-    </row>
-    <row r="31" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="W30" s="1"/>
+      <c r="X30" s="1"/>
+    </row>
+    <row r="31" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A31" s="1"/>
       <c r="B31" s="1"/>
       <c r="C31" s="1"/>
@@ -1328,8 +1451,10 @@
       <c r="T31" s="1"/>
       <c r="U31" s="1"/>
       <c r="V31" s="1"/>
-    </row>
-    <row r="32" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="W31" s="1"/>
+      <c r="X31" s="1"/>
+    </row>
+    <row r="32" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A32" s="1"/>
       <c r="B32" s="1"/>
       <c r="C32" s="1"/>
@@ -1352,8 +1477,10 @@
       <c r="T32" s="1"/>
       <c r="U32" s="1"/>
       <c r="V32" s="1"/>
-    </row>
-    <row r="33" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="W32" s="1"/>
+      <c r="X32" s="1"/>
+    </row>
+    <row r="33" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A33" s="1"/>
       <c r="B33" s="1"/>
       <c r="C33" s="1"/>
@@ -1376,8 +1503,10 @@
       <c r="T33" s="1"/>
       <c r="U33" s="1"/>
       <c r="V33" s="1"/>
-    </row>
-    <row r="34" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="W33" s="1"/>
+      <c r="X33" s="1"/>
+    </row>
+    <row r="34" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A34" s="1"/>
       <c r="B34" s="1"/>
       <c r="C34" s="1"/>
@@ -1400,8 +1529,10 @@
       <c r="T34" s="1"/>
       <c r="U34" s="1"/>
       <c r="V34" s="1"/>
-    </row>
-    <row r="35" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="W34" s="1"/>
+      <c r="X34" s="1"/>
+    </row>
+    <row r="35" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A35" s="1"/>
       <c r="B35" s="1"/>
       <c r="C35" s="1"/>
@@ -1424,8 +1555,10 @@
       <c r="T35" s="1"/>
       <c r="U35" s="1"/>
       <c r="V35" s="1"/>
-    </row>
-    <row r="36" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="W35" s="1"/>
+      <c r="X35" s="1"/>
+    </row>
+    <row r="36" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A36" s="1"/>
       <c r="B36" s="1"/>
       <c r="C36" s="1"/>
@@ -1448,8 +1581,10 @@
       <c r="T36" s="1"/>
       <c r="U36" s="1"/>
       <c r="V36" s="1"/>
-    </row>
-    <row r="37" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="W36" s="1"/>
+      <c r="X36" s="1"/>
+    </row>
+    <row r="37" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A37" s="1"/>
       <c r="B37" s="1"/>
       <c r="C37" s="1"/>
@@ -1472,8 +1607,10 @@
       <c r="T37" s="1"/>
       <c r="U37" s="1"/>
       <c r="V37" s="1"/>
-    </row>
-    <row r="38" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="W37" s="1"/>
+      <c r="X37" s="1"/>
+    </row>
+    <row r="38" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A38" s="1"/>
       <c r="B38" s="1"/>
       <c r="C38" s="1"/>
@@ -1496,8 +1633,10 @@
       <c r="T38" s="1"/>
       <c r="U38" s="1"/>
       <c r="V38" s="1"/>
-    </row>
-    <row r="39" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="W38" s="1"/>
+      <c r="X38" s="1"/>
+    </row>
+    <row r="39" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A39" s="1"/>
       <c r="B39" s="1"/>
       <c r="C39" s="1"/>
@@ -1520,8 +1659,10 @@
       <c r="T39" s="1"/>
       <c r="U39" s="1"/>
       <c r="V39" s="1"/>
-    </row>
-    <row r="40" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="W39" s="1"/>
+      <c r="X39" s="1"/>
+    </row>
+    <row r="40" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A40" s="1"/>
       <c r="B40" s="1"/>
       <c r="C40" s="1"/>
@@ -1544,8 +1685,10 @@
       <c r="T40" s="1"/>
       <c r="U40" s="1"/>
       <c r="V40" s="1"/>
-    </row>
-    <row r="41" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="W40" s="1"/>
+      <c r="X40" s="1"/>
+    </row>
+    <row r="41" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A41" s="1"/>
       <c r="B41" s="1"/>
       <c r="C41" s="1"/>
@@ -1568,8 +1711,10 @@
       <c r="T41" s="1"/>
       <c r="U41" s="1"/>
       <c r="V41" s="1"/>
-    </row>
-    <row r="42" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="W41" s="1"/>
+      <c r="X41" s="1"/>
+    </row>
+    <row r="42" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A42" s="1"/>
       <c r="B42" s="1"/>
       <c r="C42" s="1"/>
@@ -1592,8 +1737,10 @@
       <c r="T42" s="1"/>
       <c r="U42" s="1"/>
       <c r="V42" s="1"/>
-    </row>
-    <row r="43" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="W42" s="1"/>
+      <c r="X42" s="1"/>
+    </row>
+    <row r="43" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A43" s="1"/>
       <c r="B43" s="1"/>
       <c r="C43" s="1"/>
@@ -1616,8 +1763,10 @@
       <c r="T43" s="1"/>
       <c r="U43" s="1"/>
       <c r="V43" s="1"/>
-    </row>
-    <row r="44" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="W43" s="1"/>
+      <c r="X43" s="1"/>
+    </row>
+    <row r="44" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A44" s="1"/>
       <c r="B44" s="1"/>
       <c r="C44" s="1"/>
@@ -1640,8 +1789,10 @@
       <c r="T44" s="1"/>
       <c r="U44" s="1"/>
       <c r="V44" s="1"/>
-    </row>
-    <row r="45" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="W44" s="1"/>
+      <c r="X44" s="1"/>
+    </row>
+    <row r="45" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A45" s="1"/>
       <c r="B45" s="1"/>
       <c r="C45" s="1"/>
@@ -1664,8 +1815,10 @@
       <c r="T45" s="1"/>
       <c r="U45" s="1"/>
       <c r="V45" s="1"/>
-    </row>
-    <row r="46" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="W45" s="1"/>
+      <c r="X45" s="1"/>
+    </row>
+    <row r="46" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A46" s="1"/>
       <c r="B46" s="1"/>
       <c r="C46" s="1"/>
@@ -1688,8 +1841,10 @@
       <c r="T46" s="1"/>
       <c r="U46" s="1"/>
       <c r="V46" s="1"/>
-    </row>
-    <row r="47" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="W46" s="1"/>
+      <c r="X46" s="1"/>
+    </row>
+    <row r="47" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A47" s="1"/>
       <c r="B47" s="1"/>
       <c r="C47" s="1"/>
@@ -1712,8 +1867,10 @@
       <c r="T47" s="1"/>
       <c r="U47" s="1"/>
       <c r="V47" s="1"/>
-    </row>
-    <row r="48" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="W47" s="1"/>
+      <c r="X47" s="1"/>
+    </row>
+    <row r="48" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A48" s="1"/>
       <c r="B48" s="1"/>
       <c r="C48" s="1"/>
@@ -1736,8 +1893,10 @@
       <c r="T48" s="1"/>
       <c r="U48" s="1"/>
       <c r="V48" s="1"/>
-    </row>
-    <row r="49" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="W48" s="1"/>
+      <c r="X48" s="1"/>
+    </row>
+    <row r="49" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A49" s="1"/>
       <c r="B49" s="1"/>
       <c r="C49" s="1"/>
@@ -1760,8 +1919,10 @@
       <c r="T49" s="1"/>
       <c r="U49" s="1"/>
       <c r="V49" s="1"/>
-    </row>
-    <row r="50" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="W49" s="1"/>
+      <c r="X49" s="1"/>
+    </row>
+    <row r="50" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A50" s="1"/>
       <c r="B50" s="1"/>
       <c r="C50" s="1"/>
@@ -1784,8 +1945,10 @@
       <c r="T50" s="1"/>
       <c r="U50" s="1"/>
       <c r="V50" s="1"/>
-    </row>
-    <row r="51" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="W50" s="1"/>
+      <c r="X50" s="1"/>
+    </row>
+    <row r="51" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A51" s="1"/>
       <c r="B51" s="1"/>
       <c r="C51" s="1"/>
@@ -1808,8 +1971,10 @@
       <c r="T51" s="1"/>
       <c r="U51" s="1"/>
       <c r="V51" s="1"/>
-    </row>
-    <row r="52" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="W51" s="1"/>
+      <c r="X51" s="1"/>
+    </row>
+    <row r="52" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A52" s="1"/>
       <c r="B52" s="1"/>
       <c r="C52" s="1"/>
@@ -1832,8 +1997,10 @@
       <c r="T52" s="1"/>
       <c r="U52" s="1"/>
       <c r="V52" s="1"/>
-    </row>
-    <row r="53" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="W52" s="1"/>
+      <c r="X52" s="1"/>
+    </row>
+    <row r="53" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A53" s="1"/>
       <c r="B53" s="1"/>
       <c r="C53" s="1"/>
@@ -1856,8 +2023,10 @@
       <c r="T53" s="1"/>
       <c r="U53" s="1"/>
       <c r="V53" s="1"/>
-    </row>
-    <row r="54" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="W53" s="1"/>
+      <c r="X53" s="1"/>
+    </row>
+    <row r="54" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A54" s="1"/>
       <c r="B54" s="1"/>
       <c r="C54" s="1"/>
@@ -1880,8 +2049,10 @@
       <c r="T54" s="1"/>
       <c r="U54" s="1"/>
       <c r="V54" s="1"/>
-    </row>
-    <row r="55" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="W54" s="1"/>
+      <c r="X54" s="1"/>
+    </row>
+    <row r="55" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A55" s="1"/>
       <c r="B55" s="1"/>
       <c r="C55" s="1"/>
@@ -1904,8 +2075,10 @@
       <c r="T55" s="1"/>
       <c r="U55" s="1"/>
       <c r="V55" s="1"/>
-    </row>
-    <row r="56" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="W55" s="1"/>
+      <c r="X55" s="1"/>
+    </row>
+    <row r="56" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A56" s="1"/>
       <c r="B56" s="1"/>
       <c r="C56" s="1"/>
@@ -1928,8 +2101,10 @@
       <c r="T56" s="1"/>
       <c r="U56" s="1"/>
       <c r="V56" s="1"/>
-    </row>
-    <row r="57" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="W56" s="1"/>
+      <c r="X56" s="1"/>
+    </row>
+    <row r="57" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A57" s="1"/>
       <c r="B57" s="1"/>
       <c r="C57" s="1"/>
@@ -1952,8 +2127,10 @@
       <c r="T57" s="1"/>
       <c r="U57" s="1"/>
       <c r="V57" s="1"/>
-    </row>
-    <row r="58" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="W57" s="1"/>
+      <c r="X57" s="1"/>
+    </row>
+    <row r="58" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A58" s="1"/>
       <c r="B58" s="1"/>
       <c r="C58" s="1"/>
@@ -1976,8 +2153,10 @@
       <c r="T58" s="1"/>
       <c r="U58" s="1"/>
       <c r="V58" s="1"/>
-    </row>
-    <row r="59" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="W58" s="1"/>
+      <c r="X58" s="1"/>
+    </row>
+    <row r="59" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A59" s="1"/>
       <c r="B59" s="1"/>
       <c r="C59" s="1"/>
@@ -2000,8 +2179,10 @@
       <c r="T59" s="1"/>
       <c r="U59" s="1"/>
       <c r="V59" s="1"/>
-    </row>
-    <row r="60" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="W59" s="1"/>
+      <c r="X59" s="1"/>
+    </row>
+    <row r="60" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A60" s="1"/>
       <c r="B60" s="1"/>
       <c r="C60" s="1"/>
@@ -2024,8 +2205,10 @@
       <c r="T60" s="1"/>
       <c r="U60" s="1"/>
       <c r="V60" s="1"/>
-    </row>
-    <row r="61" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="W60" s="1"/>
+      <c r="X60" s="1"/>
+    </row>
+    <row r="61" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A61" s="1"/>
       <c r="B61" s="1"/>
       <c r="C61" s="1"/>
@@ -2048,8 +2231,10 @@
       <c r="T61" s="1"/>
       <c r="U61" s="1"/>
       <c r="V61" s="1"/>
-    </row>
-    <row r="62" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="W61" s="1"/>
+      <c r="X61" s="1"/>
+    </row>
+    <row r="62" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A62" s="1"/>
       <c r="B62" s="1"/>
       <c r="C62" s="1"/>
@@ -2072,8 +2257,10 @@
       <c r="T62" s="1"/>
       <c r="U62" s="1"/>
       <c r="V62" s="1"/>
-    </row>
-    <row r="63" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="W62" s="1"/>
+      <c r="X62" s="1"/>
+    </row>
+    <row r="63" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A63" s="1"/>
       <c r="B63" s="1"/>
       <c r="C63" s="1"/>
@@ -2096,8 +2283,10 @@
       <c r="T63" s="1"/>
       <c r="U63" s="1"/>
       <c r="V63" s="1"/>
-    </row>
-    <row r="64" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="W63" s="1"/>
+      <c r="X63" s="1"/>
+    </row>
+    <row r="64" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A64" s="1"/>
       <c r="B64" s="1"/>
       <c r="C64" s="1"/>
@@ -2120,8 +2309,10 @@
       <c r="T64" s="1"/>
       <c r="U64" s="1"/>
       <c r="V64" s="1"/>
-    </row>
-    <row r="65" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="W64" s="1"/>
+      <c r="X64" s="1"/>
+    </row>
+    <row r="65" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A65" s="1"/>
       <c r="B65" s="1"/>
       <c r="C65" s="1"/>
@@ -2144,8 +2335,10 @@
       <c r="T65" s="1"/>
       <c r="U65" s="1"/>
       <c r="V65" s="1"/>
-    </row>
-    <row r="66" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="W65" s="1"/>
+      <c r="X65" s="1"/>
+    </row>
+    <row r="66" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A66" s="1"/>
       <c r="B66" s="1"/>
       <c r="C66" s="1"/>
@@ -2168,8 +2361,10 @@
       <c r="T66" s="1"/>
       <c r="U66" s="1"/>
       <c r="V66" s="1"/>
-    </row>
-    <row r="67" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="W66" s="1"/>
+      <c r="X66" s="1"/>
+    </row>
+    <row r="67" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A67" s="1"/>
       <c r="B67" s="1"/>
       <c r="C67" s="1"/>
@@ -2192,8 +2387,10 @@
       <c r="T67" s="1"/>
       <c r="U67" s="1"/>
       <c r="V67" s="1"/>
-    </row>
-    <row r="68" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="W67" s="1"/>
+      <c r="X67" s="1"/>
+    </row>
+    <row r="68" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A68" s="1"/>
       <c r="B68" s="1"/>
       <c r="C68" s="1"/>
@@ -2216,8 +2413,10 @@
       <c r="T68" s="1"/>
       <c r="U68" s="1"/>
       <c r="V68" s="1"/>
-    </row>
-    <row r="69" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="W68" s="1"/>
+      <c r="X68" s="1"/>
+    </row>
+    <row r="69" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A69" s="1"/>
       <c r="B69" s="1"/>
       <c r="C69" s="1"/>
@@ -2240,8 +2439,10 @@
       <c r="T69" s="1"/>
       <c r="U69" s="1"/>
       <c r="V69" s="1"/>
-    </row>
-    <row r="70" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="W69" s="1"/>
+      <c r="X69" s="1"/>
+    </row>
+    <row r="70" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A70" s="1"/>
       <c r="B70" s="1"/>
       <c r="C70" s="1"/>
@@ -2264,8 +2465,10 @@
       <c r="T70" s="1"/>
       <c r="U70" s="1"/>
       <c r="V70" s="1"/>
-    </row>
-    <row r="71" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="W70" s="1"/>
+      <c r="X70" s="1"/>
+    </row>
+    <row r="71" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A71" s="1"/>
       <c r="B71" s="1"/>
       <c r="C71" s="1"/>
@@ -2288,8 +2491,10 @@
       <c r="T71" s="1"/>
       <c r="U71" s="1"/>
       <c r="V71" s="1"/>
-    </row>
-    <row r="72" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="W71" s="1"/>
+      <c r="X71" s="1"/>
+    </row>
+    <row r="72" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A72" s="1"/>
       <c r="B72" s="1"/>
       <c r="C72" s="1"/>
@@ -2312,8 +2517,10 @@
       <c r="T72" s="1"/>
       <c r="U72" s="1"/>
       <c r="V72" s="1"/>
-    </row>
-    <row r="73" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="W72" s="1"/>
+      <c r="X72" s="1"/>
+    </row>
+    <row r="73" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A73" s="1"/>
       <c r="B73" s="1"/>
       <c r="C73" s="1"/>
@@ -2336,8 +2543,10 @@
       <c r="T73" s="1"/>
       <c r="U73" s="1"/>
       <c r="V73" s="1"/>
-    </row>
-    <row r="74" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="W73" s="1"/>
+      <c r="X73" s="1"/>
+    </row>
+    <row r="74" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A74" s="1"/>
       <c r="B74" s="1"/>
       <c r="C74" s="1"/>
@@ -2360,8 +2569,10 @@
       <c r="T74" s="1"/>
       <c r="U74" s="1"/>
       <c r="V74" s="1"/>
-    </row>
-    <row r="75" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="W74" s="1"/>
+      <c r="X74" s="1"/>
+    </row>
+    <row r="75" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A75" s="1"/>
       <c r="B75" s="1"/>
       <c r="C75" s="1"/>
@@ -2384,8 +2595,10 @@
       <c r="T75" s="1"/>
       <c r="U75" s="1"/>
       <c r="V75" s="1"/>
-    </row>
-    <row r="76" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="W75" s="1"/>
+      <c r="X75" s="1"/>
+    </row>
+    <row r="76" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A76" s="1"/>
       <c r="B76" s="1"/>
       <c r="C76" s="1"/>
@@ -2408,8 +2621,10 @@
       <c r="T76" s="1"/>
       <c r="U76" s="1"/>
       <c r="V76" s="1"/>
-    </row>
-    <row r="77" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="W76" s="1"/>
+      <c r="X76" s="1"/>
+    </row>
+    <row r="77" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A77" s="1"/>
       <c r="B77" s="1"/>
       <c r="C77" s="1"/>
@@ -2432,8 +2647,10 @@
       <c r="T77" s="1"/>
       <c r="U77" s="1"/>
       <c r="V77" s="1"/>
-    </row>
-    <row r="78" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="W77" s="1"/>
+      <c r="X77" s="1"/>
+    </row>
+    <row r="78" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A78" s="1"/>
       <c r="B78" s="1"/>
       <c r="C78" s="1"/>
@@ -2456,8 +2673,10 @@
       <c r="T78" s="1"/>
       <c r="U78" s="1"/>
       <c r="V78" s="1"/>
-    </row>
-    <row r="79" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="W78" s="1"/>
+      <c r="X78" s="1"/>
+    </row>
+    <row r="79" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A79" s="1"/>
       <c r="B79" s="1"/>
       <c r="C79" s="1"/>
@@ -2480,8 +2699,10 @@
       <c r="T79" s="1"/>
       <c r="U79" s="1"/>
       <c r="V79" s="1"/>
-    </row>
-    <row r="80" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="W79" s="1"/>
+      <c r="X79" s="1"/>
+    </row>
+    <row r="80" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A80" s="1"/>
       <c r="B80" s="1"/>
       <c r="C80" s="1"/>
@@ -2504,8 +2725,10 @@
       <c r="T80" s="1"/>
       <c r="U80" s="1"/>
       <c r="V80" s="1"/>
-    </row>
-    <row r="81" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="W80" s="1"/>
+      <c r="X80" s="1"/>
+    </row>
+    <row r="81" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A81" s="1"/>
       <c r="B81" s="1"/>
       <c r="C81" s="1"/>
@@ -2528,8 +2751,10 @@
       <c r="T81" s="1"/>
       <c r="U81" s="1"/>
       <c r="V81" s="1"/>
-    </row>
-    <row r="82" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="W81" s="1"/>
+      <c r="X81" s="1"/>
+    </row>
+    <row r="82" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A82" s="1"/>
       <c r="B82" s="1"/>
       <c r="C82" s="1"/>
@@ -2552,8 +2777,10 @@
       <c r="T82" s="1"/>
       <c r="U82" s="1"/>
       <c r="V82" s="1"/>
-    </row>
-    <row r="83" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="W82" s="1"/>
+      <c r="X82" s="1"/>
+    </row>
+    <row r="83" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A83" s="1"/>
       <c r="B83" s="1"/>
       <c r="C83" s="1"/>
@@ -2576,8 +2803,10 @@
       <c r="T83" s="1"/>
       <c r="U83" s="1"/>
       <c r="V83" s="1"/>
-    </row>
-    <row r="84" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="W83" s="1"/>
+      <c r="X83" s="1"/>
+    </row>
+    <row r="84" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A84" s="1"/>
       <c r="B84" s="1"/>
       <c r="C84" s="1"/>
@@ -2600,8 +2829,10 @@
       <c r="T84" s="1"/>
       <c r="U84" s="1"/>
       <c r="V84" s="1"/>
-    </row>
-    <row r="85" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="W84" s="1"/>
+      <c r="X84" s="1"/>
+    </row>
+    <row r="85" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A85" s="1"/>
       <c r="B85" s="1"/>
       <c r="C85" s="1"/>
@@ -2624,8 +2855,10 @@
       <c r="T85" s="1"/>
       <c r="U85" s="1"/>
       <c r="V85" s="1"/>
-    </row>
-    <row r="86" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="W85" s="1"/>
+      <c r="X85" s="1"/>
+    </row>
+    <row r="86" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A86" s="1"/>
       <c r="B86" s="1"/>
       <c r="C86" s="1"/>
@@ -2648,8 +2881,10 @@
       <c r="T86" s="1"/>
       <c r="U86" s="1"/>
       <c r="V86" s="1"/>
-    </row>
-    <row r="87" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="W86" s="1"/>
+      <c r="X86" s="1"/>
+    </row>
+    <row r="87" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A87" s="1"/>
       <c r="B87" s="1"/>
       <c r="C87" s="1"/>
@@ -2672,8 +2907,10 @@
       <c r="T87" s="1"/>
       <c r="U87" s="1"/>
       <c r="V87" s="1"/>
-    </row>
-    <row r="88" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="W87" s="1"/>
+      <c r="X87" s="1"/>
+    </row>
+    <row r="88" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A88" s="1"/>
       <c r="B88" s="1"/>
       <c r="C88" s="1"/>
@@ -2696,8 +2933,10 @@
       <c r="T88" s="1"/>
       <c r="U88" s="1"/>
       <c r="V88" s="1"/>
-    </row>
-    <row r="89" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="W88" s="1"/>
+      <c r="X88" s="1"/>
+    </row>
+    <row r="89" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A89" s="1"/>
       <c r="B89" s="1"/>
       <c r="C89" s="1"/>
@@ -2720,8 +2959,10 @@
       <c r="T89" s="1"/>
       <c r="U89" s="1"/>
       <c r="V89" s="1"/>
-    </row>
-    <row r="90" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="W89" s="1"/>
+      <c r="X89" s="1"/>
+    </row>
+    <row r="90" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A90" s="1"/>
       <c r="B90" s="1"/>
       <c r="C90" s="1"/>
@@ -2744,8 +2985,10 @@
       <c r="T90" s="1"/>
       <c r="U90" s="1"/>
       <c r="V90" s="1"/>
-    </row>
-    <row r="91" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="W90" s="1"/>
+      <c r="X90" s="1"/>
+    </row>
+    <row r="91" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A91" s="1"/>
       <c r="B91" s="1"/>
       <c r="C91" s="1"/>
@@ -2768,8 +3011,10 @@
       <c r="T91" s="1"/>
       <c r="U91" s="1"/>
       <c r="V91" s="1"/>
-    </row>
-    <row r="92" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="W91" s="1"/>
+      <c r="X91" s="1"/>
+    </row>
+    <row r="92" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A92" s="1"/>
       <c r="B92" s="1"/>
       <c r="C92" s="1"/>
@@ -2792,8 +3037,10 @@
       <c r="T92" s="1"/>
       <c r="U92" s="1"/>
       <c r="V92" s="1"/>
-    </row>
-    <row r="93" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="W92" s="1"/>
+      <c r="X92" s="1"/>
+    </row>
+    <row r="93" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A93" s="1"/>
       <c r="B93" s="1"/>
       <c r="C93" s="1"/>
@@ -2816,8 +3063,10 @@
       <c r="T93" s="1"/>
       <c r="U93" s="1"/>
       <c r="V93" s="1"/>
-    </row>
-    <row r="94" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="W93" s="1"/>
+      <c r="X93" s="1"/>
+    </row>
+    <row r="94" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A94" s="1"/>
       <c r="B94" s="1"/>
       <c r="C94" s="1"/>
@@ -2840,8 +3089,10 @@
       <c r="T94" s="1"/>
       <c r="U94" s="1"/>
       <c r="V94" s="1"/>
-    </row>
-    <row r="95" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="W94" s="1"/>
+      <c r="X94" s="1"/>
+    </row>
+    <row r="95" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A95" s="1"/>
       <c r="B95" s="1"/>
       <c r="C95" s="1"/>
@@ -2864,8 +3115,10 @@
       <c r="T95" s="1"/>
       <c r="U95" s="1"/>
       <c r="V95" s="1"/>
-    </row>
-    <row r="96" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="W95" s="1"/>
+      <c r="X95" s="1"/>
+    </row>
+    <row r="96" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A96" s="1"/>
       <c r="B96" s="1"/>
       <c r="C96" s="1"/>
@@ -2888,8 +3141,10 @@
       <c r="T96" s="1"/>
       <c r="U96" s="1"/>
       <c r="V96" s="1"/>
-    </row>
-    <row r="97" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="W96" s="1"/>
+      <c r="X96" s="1"/>
+    </row>
+    <row r="97" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A97" s="1"/>
       <c r="B97" s="1"/>
       <c r="C97" s="1"/>
@@ -2912,8 +3167,10 @@
       <c r="T97" s="1"/>
       <c r="U97" s="1"/>
       <c r="V97" s="1"/>
-    </row>
-    <row r="98" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="W97" s="1"/>
+      <c r="X97" s="1"/>
+    </row>
+    <row r="98" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A98" s="1"/>
       <c r="B98" s="1"/>
       <c r="C98" s="1"/>
@@ -2936,8 +3193,10 @@
       <c r="T98" s="1"/>
       <c r="U98" s="1"/>
       <c r="V98" s="1"/>
-    </row>
-    <row r="99" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="W98" s="1"/>
+      <c r="X98" s="1"/>
+    </row>
+    <row r="99" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A99" s="1"/>
       <c r="B99" s="1"/>
       <c r="C99" s="1"/>
@@ -2960,8 +3219,10 @@
       <c r="T99" s="1"/>
       <c r="U99" s="1"/>
       <c r="V99" s="1"/>
-    </row>
-    <row r="100" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="W99" s="1"/>
+      <c r="X99" s="1"/>
+    </row>
+    <row r="100" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A100" s="1"/>
       <c r="B100" s="1"/>
       <c r="C100" s="1"/>
@@ -2984,8 +3245,10 @@
       <c r="T100" s="1"/>
       <c r="U100" s="1"/>
       <c r="V100" s="1"/>
-    </row>
-    <row r="101" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="W100" s="1"/>
+      <c r="X100" s="1"/>
+    </row>
+    <row r="101" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A101" s="1"/>
       <c r="B101" s="1"/>
       <c r="C101" s="1"/>
@@ -3008,8 +3271,10 @@
       <c r="T101" s="1"/>
       <c r="U101" s="1"/>
       <c r="V101" s="1"/>
-    </row>
-    <row r="102" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="W101" s="1"/>
+      <c r="X101" s="1"/>
+    </row>
+    <row r="102" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A102" s="1"/>
       <c r="B102" s="1"/>
       <c r="C102" s="1"/>
@@ -3032,8 +3297,10 @@
       <c r="T102" s="1"/>
       <c r="U102" s="1"/>
       <c r="V102" s="1"/>
-    </row>
-    <row r="103" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="W102" s="1"/>
+      <c r="X102" s="1"/>
+    </row>
+    <row r="103" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A103" s="1"/>
       <c r="B103" s="1"/>
       <c r="C103" s="1"/>
@@ -3056,8 +3323,10 @@
       <c r="T103" s="1"/>
       <c r="U103" s="1"/>
       <c r="V103" s="1"/>
-    </row>
-    <row r="104" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="W103" s="1"/>
+      <c r="X103" s="1"/>
+    </row>
+    <row r="104" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A104" s="1"/>
       <c r="B104" s="1"/>
       <c r="C104" s="1"/>
@@ -3080,8 +3349,10 @@
       <c r="T104" s="1"/>
       <c r="U104" s="1"/>
       <c r="V104" s="1"/>
-    </row>
-    <row r="105" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="W104" s="1"/>
+      <c r="X104" s="1"/>
+    </row>
+    <row r="105" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A105" s="1"/>
       <c r="B105" s="1"/>
       <c r="C105" s="1"/>
@@ -3104,8 +3375,10 @@
       <c r="T105" s="1"/>
       <c r="U105" s="1"/>
       <c r="V105" s="1"/>
-    </row>
-    <row r="106" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="W105" s="1"/>
+      <c r="X105" s="1"/>
+    </row>
+    <row r="106" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A106" s="1"/>
       <c r="B106" s="1"/>
       <c r="C106" s="1"/>
@@ -3128,8 +3401,10 @@
       <c r="T106" s="1"/>
       <c r="U106" s="1"/>
       <c r="V106" s="1"/>
-    </row>
-    <row r="107" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="W106" s="1"/>
+      <c r="X106" s="1"/>
+    </row>
+    <row r="107" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A107" s="1"/>
       <c r="B107" s="1"/>
       <c r="C107" s="1"/>
@@ -3152,8 +3427,10 @@
       <c r="T107" s="1"/>
       <c r="U107" s="1"/>
       <c r="V107" s="1"/>
-    </row>
-    <row r="108" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="W107" s="1"/>
+      <c r="X107" s="1"/>
+    </row>
+    <row r="108" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A108" s="1"/>
       <c r="B108" s="1"/>
       <c r="C108" s="1"/>
@@ -3176,8 +3453,10 @@
       <c r="T108" s="1"/>
       <c r="U108" s="1"/>
       <c r="V108" s="1"/>
-    </row>
-    <row r="109" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="W108" s="1"/>
+      <c r="X108" s="1"/>
+    </row>
+    <row r="109" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A109" s="1"/>
       <c r="B109" s="1"/>
       <c r="C109" s="1"/>
@@ -3200,8 +3479,10 @@
       <c r="T109" s="1"/>
       <c r="U109" s="1"/>
       <c r="V109" s="1"/>
-    </row>
-    <row r="110" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="W109" s="1"/>
+      <c r="X109" s="1"/>
+    </row>
+    <row r="110" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A110" s="1"/>
       <c r="B110" s="1"/>
       <c r="C110" s="1"/>
@@ -3224,8 +3505,10 @@
       <c r="T110" s="1"/>
       <c r="U110" s="1"/>
       <c r="V110" s="1"/>
-    </row>
-    <row r="111" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="W110" s="1"/>
+      <c r="X110" s="1"/>
+    </row>
+    <row r="111" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A111" s="1"/>
       <c r="B111" s="1"/>
       <c r="C111" s="1"/>
@@ -3248,8 +3531,10 @@
       <c r="T111" s="1"/>
       <c r="U111" s="1"/>
       <c r="V111" s="1"/>
-    </row>
-    <row r="112" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="W111" s="1"/>
+      <c r="X111" s="1"/>
+    </row>
+    <row r="112" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A112" s="1"/>
       <c r="B112" s="1"/>
       <c r="C112" s="1"/>
@@ -3272,8 +3557,10 @@
       <c r="T112" s="1"/>
       <c r="U112" s="1"/>
       <c r="V112" s="1"/>
-    </row>
-    <row r="113" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="W112" s="1"/>
+      <c r="X112" s="1"/>
+    </row>
+    <row r="113" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A113" s="1"/>
       <c r="B113" s="1"/>
       <c r="C113" s="1"/>
@@ -3296,8 +3583,10 @@
       <c r="T113" s="1"/>
       <c r="U113" s="1"/>
       <c r="V113" s="1"/>
-    </row>
-    <row r="114" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="W113" s="1"/>
+      <c r="X113" s="1"/>
+    </row>
+    <row r="114" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A114" s="1"/>
       <c r="B114" s="1"/>
       <c r="C114" s="1"/>
@@ -3320,8 +3609,10 @@
       <c r="T114" s="1"/>
       <c r="U114" s="1"/>
       <c r="V114" s="1"/>
-    </row>
-    <row r="115" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="W114" s="1"/>
+      <c r="X114" s="1"/>
+    </row>
+    <row r="115" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A115" s="1"/>
       <c r="B115" s="1"/>
       <c r="C115" s="1"/>
@@ -3344,8 +3635,10 @@
       <c r="T115" s="1"/>
       <c r="U115" s="1"/>
       <c r="V115" s="1"/>
-    </row>
-    <row r="116" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="W115" s="1"/>
+      <c r="X115" s="1"/>
+    </row>
+    <row r="116" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A116" s="1"/>
       <c r="B116" s="1"/>
       <c r="C116" s="1"/>
@@ -3368,8 +3661,10 @@
       <c r="T116" s="1"/>
       <c r="U116" s="1"/>
       <c r="V116" s="1"/>
-    </row>
-    <row r="117" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="W116" s="1"/>
+      <c r="X116" s="1"/>
+    </row>
+    <row r="117" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A117" s="1"/>
       <c r="B117" s="1"/>
       <c r="C117" s="1"/>
@@ -3392,8 +3687,10 @@
       <c r="T117" s="1"/>
       <c r="U117" s="1"/>
       <c r="V117" s="1"/>
-    </row>
-    <row r="118" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="W117" s="1"/>
+      <c r="X117" s="1"/>
+    </row>
+    <row r="118" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A118" s="1"/>
       <c r="B118" s="1"/>
       <c r="C118" s="1"/>
@@ -3416,8 +3713,10 @@
       <c r="T118" s="1"/>
       <c r="U118" s="1"/>
       <c r="V118" s="1"/>
-    </row>
-    <row r="119" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="W118" s="1"/>
+      <c r="X118" s="1"/>
+    </row>
+    <row r="119" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A119" s="1"/>
       <c r="B119" s="1"/>
       <c r="C119" s="1"/>
@@ -3440,8 +3739,10 @@
       <c r="T119" s="1"/>
       <c r="U119" s="1"/>
       <c r="V119" s="1"/>
-    </row>
-    <row r="120" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="W119" s="1"/>
+      <c r="X119" s="1"/>
+    </row>
+    <row r="120" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A120" s="1"/>
       <c r="B120" s="1"/>
       <c r="C120" s="1"/>
@@ -3464,8 +3765,10 @@
       <c r="T120" s="1"/>
       <c r="U120" s="1"/>
       <c r="V120" s="1"/>
-    </row>
-    <row r="121" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="W120" s="1"/>
+      <c r="X120" s="1"/>
+    </row>
+    <row r="121" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A121" s="1"/>
       <c r="B121" s="1"/>
       <c r="C121" s="1"/>
@@ -3488,8 +3791,10 @@
       <c r="T121" s="1"/>
       <c r="U121" s="1"/>
       <c r="V121" s="1"/>
-    </row>
-    <row r="122" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="W121" s="1"/>
+      <c r="X121" s="1"/>
+    </row>
+    <row r="122" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A122" s="1"/>
       <c r="B122" s="1"/>
       <c r="C122" s="1"/>
@@ -3512,8 +3817,10 @@
       <c r="T122" s="1"/>
       <c r="U122" s="1"/>
       <c r="V122" s="1"/>
-    </row>
-    <row r="123" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="W122" s="1"/>
+      <c r="X122" s="1"/>
+    </row>
+    <row r="123" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A123" s="1"/>
       <c r="B123" s="1"/>
       <c r="C123" s="1"/>
@@ -3536,8 +3843,10 @@
       <c r="T123" s="1"/>
       <c r="U123" s="1"/>
       <c r="V123" s="1"/>
-    </row>
-    <row r="124" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="W123" s="1"/>
+      <c r="X123" s="1"/>
+    </row>
+    <row r="124" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A124" s="1"/>
       <c r="B124" s="1"/>
       <c r="C124" s="1"/>
@@ -3560,8 +3869,10 @@
       <c r="T124" s="1"/>
       <c r="U124" s="1"/>
       <c r="V124" s="1"/>
-    </row>
-    <row r="125" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="W124" s="1"/>
+      <c r="X124" s="1"/>
+    </row>
+    <row r="125" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A125" s="1"/>
       <c r="B125" s="1"/>
       <c r="C125" s="1"/>
@@ -3584,8 +3895,10 @@
       <c r="T125" s="1"/>
       <c r="U125" s="1"/>
       <c r="V125" s="1"/>
-    </row>
-    <row r="126" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="W125" s="1"/>
+      <c r="X125" s="1"/>
+    </row>
+    <row r="126" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A126" s="1"/>
       <c r="B126" s="1"/>
       <c r="C126" s="1"/>
@@ -3608,8 +3921,10 @@
       <c r="T126" s="1"/>
       <c r="U126" s="1"/>
       <c r="V126" s="1"/>
-    </row>
-    <row r="127" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="W126" s="1"/>
+      <c r="X126" s="1"/>
+    </row>
+    <row r="127" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A127" s="1"/>
       <c r="B127" s="1"/>
       <c r="C127" s="1"/>
@@ -3632,8 +3947,10 @@
       <c r="T127" s="1"/>
       <c r="U127" s="1"/>
       <c r="V127" s="1"/>
-    </row>
-    <row r="128" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="W127" s="1"/>
+      <c r="X127" s="1"/>
+    </row>
+    <row r="128" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A128" s="1"/>
       <c r="B128" s="1"/>
       <c r="C128" s="1"/>
@@ -3656,8 +3973,10 @@
       <c r="T128" s="1"/>
       <c r="U128" s="1"/>
       <c r="V128" s="1"/>
-    </row>
-    <row r="129" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="W128" s="1"/>
+      <c r="X128" s="1"/>
+    </row>
+    <row r="129" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A129" s="1"/>
       <c r="B129" s="1"/>
       <c r="C129" s="1"/>
@@ -3680,8 +3999,10 @@
       <c r="T129" s="1"/>
       <c r="U129" s="1"/>
       <c r="V129" s="1"/>
-    </row>
-    <row r="130" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="W129" s="1"/>
+      <c r="X129" s="1"/>
+    </row>
+    <row r="130" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A130" s="1"/>
       <c r="B130" s="1"/>
       <c r="C130" s="1"/>
@@ -3704,8 +4025,10 @@
       <c r="T130" s="1"/>
       <c r="U130" s="1"/>
       <c r="V130" s="1"/>
-    </row>
-    <row r="131" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="W130" s="1"/>
+      <c r="X130" s="1"/>
+    </row>
+    <row r="131" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A131" s="1"/>
       <c r="B131" s="1"/>
       <c r="C131" s="1"/>
@@ -3728,8 +4051,10 @@
       <c r="T131" s="1"/>
       <c r="U131" s="1"/>
       <c r="V131" s="1"/>
-    </row>
-    <row r="132" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="W131" s="1"/>
+      <c r="X131" s="1"/>
+    </row>
+    <row r="132" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A132" s="1"/>
       <c r="B132" s="1"/>
       <c r="C132" s="1"/>
@@ -3752,8 +4077,10 @@
       <c r="T132" s="1"/>
       <c r="U132" s="1"/>
       <c r="V132" s="1"/>
-    </row>
-    <row r="133" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="W132" s="1"/>
+      <c r="X132" s="1"/>
+    </row>
+    <row r="133" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A133" s="1"/>
       <c r="B133" s="1"/>
       <c r="C133" s="1"/>
@@ -3776,8 +4103,10 @@
       <c r="T133" s="1"/>
       <c r="U133" s="1"/>
       <c r="V133" s="1"/>
-    </row>
-    <row r="134" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="W133" s="1"/>
+      <c r="X133" s="1"/>
+    </row>
+    <row r="134" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A134" s="1"/>
       <c r="B134" s="1"/>
       <c r="C134" s="1"/>
@@ -3800,8 +4129,10 @@
       <c r="T134" s="1"/>
       <c r="U134" s="1"/>
       <c r="V134" s="1"/>
-    </row>
-    <row r="135" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="W134" s="1"/>
+      <c r="X134" s="1"/>
+    </row>
+    <row r="135" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A135" s="1"/>
       <c r="B135" s="1"/>
       <c r="C135" s="1"/>
@@ -3824,8 +4155,10 @@
       <c r="T135" s="1"/>
       <c r="U135" s="1"/>
       <c r="V135" s="1"/>
-    </row>
-    <row r="136" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="W135" s="1"/>
+      <c r="X135" s="1"/>
+    </row>
+    <row r="136" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A136" s="1"/>
       <c r="B136" s="1"/>
       <c r="C136" s="1"/>
@@ -3848,8 +4181,10 @@
       <c r="T136" s="1"/>
       <c r="U136" s="1"/>
       <c r="V136" s="1"/>
-    </row>
-    <row r="137" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="W136" s="1"/>
+      <c r="X136" s="1"/>
+    </row>
+    <row r="137" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A137" s="1"/>
       <c r="B137" s="1"/>
       <c r="C137" s="1"/>
@@ -3872,8 +4207,10 @@
       <c r="T137" s="1"/>
       <c r="U137" s="1"/>
       <c r="V137" s="1"/>
-    </row>
-    <row r="138" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="W137" s="1"/>
+      <c r="X137" s="1"/>
+    </row>
+    <row r="138" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A138" s="1"/>
       <c r="B138" s="1"/>
       <c r="C138" s="1"/>
@@ -3896,8 +4233,10 @@
       <c r="T138" s="1"/>
       <c r="U138" s="1"/>
       <c r="V138" s="1"/>
-    </row>
-    <row r="139" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="W138" s="1"/>
+      <c r="X138" s="1"/>
+    </row>
+    <row r="139" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A139" s="1"/>
       <c r="B139" s="1"/>
       <c r="C139" s="1"/>
@@ -3920,8 +4259,10 @@
       <c r="T139" s="1"/>
       <c r="U139" s="1"/>
       <c r="V139" s="1"/>
-    </row>
-    <row r="140" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="W139" s="1"/>
+      <c r="X139" s="1"/>
+    </row>
+    <row r="140" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A140" s="1"/>
       <c r="B140" s="1"/>
       <c r="C140" s="1"/>
@@ -3944,8 +4285,10 @@
       <c r="T140" s="1"/>
       <c r="U140" s="1"/>
       <c r="V140" s="1"/>
-    </row>
-    <row r="141" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="W140" s="1"/>
+      <c r="X140" s="1"/>
+    </row>
+    <row r="141" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A141" s="1"/>
       <c r="B141" s="1"/>
       <c r="C141" s="1"/>
@@ -3968,8 +4311,10 @@
       <c r="T141" s="1"/>
       <c r="U141" s="1"/>
       <c r="V141" s="1"/>
-    </row>
-    <row r="142" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="W141" s="1"/>
+      <c r="X141" s="1"/>
+    </row>
+    <row r="142" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A142" s="1"/>
       <c r="B142" s="1"/>
       <c r="C142" s="1"/>
@@ -3992,8 +4337,10 @@
       <c r="T142" s="1"/>
       <c r="U142" s="1"/>
       <c r="V142" s="1"/>
-    </row>
-    <row r="143" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="W142" s="1"/>
+      <c r="X142" s="1"/>
+    </row>
+    <row r="143" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A143" s="1"/>
       <c r="B143" s="1"/>
       <c r="C143" s="1"/>
@@ -4016,8 +4363,10 @@
       <c r="T143" s="1"/>
       <c r="U143" s="1"/>
       <c r="V143" s="1"/>
-    </row>
-    <row r="144" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="W143" s="1"/>
+      <c r="X143" s="1"/>
+    </row>
+    <row r="144" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A144" s="1"/>
       <c r="B144" s="1"/>
       <c r="C144" s="1"/>
@@ -4040,8 +4389,10 @@
       <c r="T144" s="1"/>
       <c r="U144" s="1"/>
       <c r="V144" s="1"/>
-    </row>
-    <row r="145" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="W144" s="1"/>
+      <c r="X144" s="1"/>
+    </row>
+    <row r="145" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A145" s="1"/>
       <c r="B145" s="1"/>
       <c r="C145" s="1"/>
@@ -4064,8 +4415,10 @@
       <c r="T145" s="1"/>
       <c r="U145" s="1"/>
       <c r="V145" s="1"/>
-    </row>
-    <row r="146" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="W145" s="1"/>
+      <c r="X145" s="1"/>
+    </row>
+    <row r="146" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A146" s="1"/>
       <c r="B146" s="1"/>
       <c r="C146" s="1"/>
@@ -4088,8 +4441,10 @@
       <c r="T146" s="1"/>
       <c r="U146" s="1"/>
       <c r="V146" s="1"/>
-    </row>
-    <row r="147" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="W146" s="1"/>
+      <c r="X146" s="1"/>
+    </row>
+    <row r="147" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A147" s="1"/>
       <c r="B147" s="1"/>
       <c r="C147" s="1"/>
@@ -4112,8 +4467,10 @@
       <c r="T147" s="1"/>
       <c r="U147" s="1"/>
       <c r="V147" s="1"/>
-    </row>
-    <row r="148" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="W147" s="1"/>
+      <c r="X147" s="1"/>
+    </row>
+    <row r="148" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A148" s="1"/>
       <c r="B148" s="1"/>
       <c r="C148" s="1"/>
@@ -4136,8 +4493,10 @@
       <c r="T148" s="1"/>
       <c r="U148" s="1"/>
       <c r="V148" s="1"/>
-    </row>
-    <row r="149" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="W148" s="1"/>
+      <c r="X148" s="1"/>
+    </row>
+    <row r="149" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A149" s="1"/>
       <c r="B149" s="1"/>
       <c r="C149" s="1"/>
@@ -4160,8 +4519,10 @@
       <c r="T149" s="1"/>
       <c r="U149" s="1"/>
       <c r="V149" s="1"/>
-    </row>
-    <row r="150" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="W149" s="1"/>
+      <c r="X149" s="1"/>
+    </row>
+    <row r="150" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A150" s="1"/>
       <c r="B150" s="1"/>
       <c r="C150" s="1"/>
@@ -4184,8 +4545,10 @@
       <c r="T150" s="1"/>
       <c r="U150" s="1"/>
       <c r="V150" s="1"/>
-    </row>
-    <row r="151" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="W150" s="1"/>
+      <c r="X150" s="1"/>
+    </row>
+    <row r="151" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A151" s="1"/>
       <c r="B151" s="1"/>
       <c r="C151" s="1"/>
@@ -4208,8 +4571,10 @@
       <c r="T151" s="1"/>
       <c r="U151" s="1"/>
       <c r="V151" s="1"/>
-    </row>
-    <row r="152" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="W151" s="1"/>
+      <c r="X151" s="1"/>
+    </row>
+    <row r="152" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A152" s="1"/>
       <c r="B152" s="1"/>
       <c r="C152" s="1"/>
@@ -4232,8 +4597,10 @@
       <c r="T152" s="1"/>
       <c r="U152" s="1"/>
       <c r="V152" s="1"/>
-    </row>
-    <row r="153" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="W152" s="1"/>
+      <c r="X152" s="1"/>
+    </row>
+    <row r="153" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A153" s="1"/>
       <c r="B153" s="1"/>
       <c r="C153" s="1"/>
@@ -4256,8 +4623,10 @@
       <c r="T153" s="1"/>
       <c r="U153" s="1"/>
       <c r="V153" s="1"/>
-    </row>
-    <row r="154" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="W153" s="1"/>
+      <c r="X153" s="1"/>
+    </row>
+    <row r="154" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A154" s="1"/>
       <c r="B154" s="1"/>
       <c r="C154" s="1"/>
@@ -4280,8 +4649,10 @@
       <c r="T154" s="1"/>
       <c r="U154" s="1"/>
       <c r="V154" s="1"/>
-    </row>
-    <row r="155" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="W154" s="1"/>
+      <c r="X154" s="1"/>
+    </row>
+    <row r="155" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A155" s="1"/>
       <c r="B155" s="1"/>
       <c r="C155" s="1"/>
@@ -4304,8 +4675,10 @@
       <c r="T155" s="1"/>
       <c r="U155" s="1"/>
       <c r="V155" s="1"/>
-    </row>
-    <row r="156" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="W155" s="1"/>
+      <c r="X155" s="1"/>
+    </row>
+    <row r="156" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A156" s="1"/>
       <c r="B156" s="1"/>
       <c r="C156" s="1"/>
@@ -4328,8 +4701,10 @@
       <c r="T156" s="1"/>
       <c r="U156" s="1"/>
       <c r="V156" s="1"/>
-    </row>
-    <row r="157" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="W156" s="1"/>
+      <c r="X156" s="1"/>
+    </row>
+    <row r="157" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A157" s="1"/>
       <c r="B157" s="1"/>
       <c r="C157" s="1"/>
@@ -4352,8 +4727,10 @@
       <c r="T157" s="1"/>
       <c r="U157" s="1"/>
       <c r="V157" s="1"/>
-    </row>
-    <row r="158" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="W157" s="1"/>
+      <c r="X157" s="1"/>
+    </row>
+    <row r="158" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A158" s="1"/>
       <c r="B158" s="1"/>
       <c r="C158" s="1"/>
@@ -4376,8 +4753,10 @@
       <c r="T158" s="1"/>
       <c r="U158" s="1"/>
       <c r="V158" s="1"/>
-    </row>
-    <row r="159" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="W158" s="1"/>
+      <c r="X158" s="1"/>
+    </row>
+    <row r="159" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A159" s="1"/>
       <c r="B159" s="1"/>
       <c r="C159" s="1"/>
@@ -4400,8 +4779,10 @@
       <c r="T159" s="1"/>
       <c r="U159" s="1"/>
       <c r="V159" s="1"/>
-    </row>
-    <row r="160" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="W159" s="1"/>
+      <c r="X159" s="1"/>
+    </row>
+    <row r="160" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A160" s="1"/>
       <c r="B160" s="1"/>
       <c r="C160" s="1"/>
@@ -4424,8 +4805,10 @@
       <c r="T160" s="1"/>
       <c r="U160" s="1"/>
       <c r="V160" s="1"/>
-    </row>
-    <row r="161" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="W160" s="1"/>
+      <c r="X160" s="1"/>
+    </row>
+    <row r="161" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A161" s="1"/>
       <c r="B161" s="1"/>
       <c r="C161" s="1"/>
@@ -4448,8 +4831,10 @@
       <c r="T161" s="1"/>
       <c r="U161" s="1"/>
       <c r="V161" s="1"/>
-    </row>
-    <row r="162" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="W161" s="1"/>
+      <c r="X161" s="1"/>
+    </row>
+    <row r="162" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A162" s="1"/>
       <c r="B162" s="1"/>
       <c r="C162" s="1"/>
@@ -4472,8 +4857,10 @@
       <c r="T162" s="1"/>
       <c r="U162" s="1"/>
       <c r="V162" s="1"/>
-    </row>
-    <row r="163" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="W162" s="1"/>
+      <c r="X162" s="1"/>
+    </row>
+    <row r="163" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A163" s="1"/>
       <c r="B163" s="1"/>
       <c r="C163" s="1"/>
@@ -4496,8 +4883,10 @@
       <c r="T163" s="1"/>
       <c r="U163" s="1"/>
       <c r="V163" s="1"/>
-    </row>
-    <row r="164" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="W163" s="1"/>
+      <c r="X163" s="1"/>
+    </row>
+    <row r="164" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A164" s="1"/>
       <c r="B164" s="1"/>
       <c r="C164" s="1"/>
@@ -4520,8 +4909,10 @@
       <c r="T164" s="1"/>
       <c r="U164" s="1"/>
       <c r="V164" s="1"/>
-    </row>
-    <row r="165" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="W164" s="1"/>
+      <c r="X164" s="1"/>
+    </row>
+    <row r="165" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A165" s="1"/>
       <c r="B165" s="1"/>
       <c r="C165" s="1"/>
@@ -4544,8 +4935,10 @@
       <c r="T165" s="1"/>
       <c r="U165" s="1"/>
       <c r="V165" s="1"/>
-    </row>
-    <row r="166" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="W165" s="1"/>
+      <c r="X165" s="1"/>
+    </row>
+    <row r="166" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A166" s="1"/>
       <c r="B166" s="1"/>
       <c r="C166" s="1"/>
@@ -4568,8 +4961,10 @@
       <c r="T166" s="1"/>
       <c r="U166" s="1"/>
       <c r="V166" s="1"/>
-    </row>
-    <row r="167" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="W166" s="1"/>
+      <c r="X166" s="1"/>
+    </row>
+    <row r="167" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A167" s="1"/>
       <c r="B167" s="1"/>
       <c r="C167" s="1"/>
@@ -4592,8 +4987,10 @@
       <c r="T167" s="1"/>
       <c r="U167" s="1"/>
       <c r="V167" s="1"/>
-    </row>
-    <row r="168" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="W167" s="1"/>
+      <c r="X167" s="1"/>
+    </row>
+    <row r="168" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A168" s="1"/>
       <c r="B168" s="1"/>
       <c r="C168" s="1"/>
@@ -4616,8 +5013,10 @@
       <c r="T168" s="1"/>
       <c r="U168" s="1"/>
       <c r="V168" s="1"/>
-    </row>
-    <row r="169" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="W168" s="1"/>
+      <c r="X168" s="1"/>
+    </row>
+    <row r="169" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A169" s="1"/>
       <c r="B169" s="1"/>
       <c r="C169" s="1"/>
@@ -4640,8 +5039,10 @@
       <c r="T169" s="1"/>
       <c r="U169" s="1"/>
       <c r="V169" s="1"/>
-    </row>
-    <row r="170" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="W169" s="1"/>
+      <c r="X169" s="1"/>
+    </row>
+    <row r="170" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A170" s="1"/>
       <c r="B170" s="1"/>
       <c r="C170" s="1"/>
@@ -4664,8 +5065,10 @@
       <c r="T170" s="1"/>
       <c r="U170" s="1"/>
       <c r="V170" s="1"/>
-    </row>
-    <row r="171" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="W170" s="1"/>
+      <c r="X170" s="1"/>
+    </row>
+    <row r="171" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A171" s="1"/>
       <c r="B171" s="1"/>
       <c r="C171" s="1"/>
@@ -4688,8 +5091,10 @@
       <c r="T171" s="1"/>
       <c r="U171" s="1"/>
       <c r="V171" s="1"/>
-    </row>
-    <row r="172" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="W171" s="1"/>
+      <c r="X171" s="1"/>
+    </row>
+    <row r="172" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A172" s="1"/>
       <c r="B172" s="1"/>
       <c r="C172" s="1"/>
@@ -4712,8 +5117,10 @@
       <c r="T172" s="1"/>
       <c r="U172" s="1"/>
       <c r="V172" s="1"/>
-    </row>
-    <row r="173" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="W172" s="1"/>
+      <c r="X172" s="1"/>
+    </row>
+    <row r="173" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A173" s="1"/>
       <c r="B173" s="1"/>
       <c r="C173" s="1"/>
@@ -4736,8 +5143,10 @@
       <c r="T173" s="1"/>
       <c r="U173" s="1"/>
       <c r="V173" s="1"/>
-    </row>
-    <row r="174" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="W173" s="1"/>
+      <c r="X173" s="1"/>
+    </row>
+    <row r="174" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A174" s="1"/>
       <c r="B174" s="1"/>
       <c r="C174" s="1"/>
@@ -4760,8 +5169,10 @@
       <c r="T174" s="1"/>
       <c r="U174" s="1"/>
       <c r="V174" s="1"/>
-    </row>
-    <row r="175" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="W174" s="1"/>
+      <c r="X174" s="1"/>
+    </row>
+    <row r="175" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A175" s="1"/>
       <c r="B175" s="1"/>
       <c r="C175" s="1"/>
@@ -4784,8 +5195,10 @@
       <c r="T175" s="1"/>
       <c r="U175" s="1"/>
       <c r="V175" s="1"/>
-    </row>
-    <row r="176" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="W175" s="1"/>
+      <c r="X175" s="1"/>
+    </row>
+    <row r="176" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A176" s="1"/>
       <c r="B176" s="1"/>
       <c r="C176" s="1"/>
@@ -4808,8 +5221,10 @@
       <c r="T176" s="1"/>
       <c r="U176" s="1"/>
       <c r="V176" s="1"/>
-    </row>
-    <row r="177" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="W176" s="1"/>
+      <c r="X176" s="1"/>
+    </row>
+    <row r="177" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A177" s="1"/>
       <c r="B177" s="1"/>
       <c r="C177" s="1"/>
@@ -4832,8 +5247,10 @@
       <c r="T177" s="1"/>
       <c r="U177" s="1"/>
       <c r="V177" s="1"/>
-    </row>
-    <row r="178" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="W177" s="1"/>
+      <c r="X177" s="1"/>
+    </row>
+    <row r="178" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A178" s="1"/>
       <c r="B178" s="1"/>
       <c r="C178" s="1"/>
@@ -4856,8 +5273,10 @@
       <c r="T178" s="1"/>
       <c r="U178" s="1"/>
       <c r="V178" s="1"/>
-    </row>
-    <row r="179" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="W178" s="1"/>
+      <c r="X178" s="1"/>
+    </row>
+    <row r="179" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A179" s="1"/>
       <c r="B179" s="1"/>
       <c r="C179" s="1"/>
@@ -4880,8 +5299,10 @@
       <c r="T179" s="1"/>
       <c r="U179" s="1"/>
       <c r="V179" s="1"/>
-    </row>
-    <row r="180" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="W179" s="1"/>
+      <c r="X179" s="1"/>
+    </row>
+    <row r="180" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A180" s="1"/>
       <c r="B180" s="1"/>
       <c r="C180" s="1"/>
@@ -4904,8 +5325,10 @@
       <c r="T180" s="1"/>
       <c r="U180" s="1"/>
       <c r="V180" s="1"/>
-    </row>
-    <row r="181" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="W180" s="1"/>
+      <c r="X180" s="1"/>
+    </row>
+    <row r="181" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A181" s="1"/>
       <c r="B181" s="1"/>
       <c r="C181" s="1"/>
@@ -4928,8 +5351,10 @@
       <c r="T181" s="1"/>
       <c r="U181" s="1"/>
       <c r="V181" s="1"/>
-    </row>
-    <row r="182" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="W181" s="1"/>
+      <c r="X181" s="1"/>
+    </row>
+    <row r="182" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A182" s="1"/>
       <c r="B182" s="1"/>
       <c r="C182" s="1"/>
@@ -4952,8 +5377,10 @@
       <c r="T182" s="1"/>
       <c r="U182" s="1"/>
       <c r="V182" s="1"/>
-    </row>
-    <row r="183" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="W182" s="1"/>
+      <c r="X182" s="1"/>
+    </row>
+    <row r="183" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A183" s="1"/>
       <c r="B183" s="1"/>
       <c r="C183" s="1"/>
@@ -4976,8 +5403,10 @@
       <c r="T183" s="1"/>
       <c r="U183" s="1"/>
       <c r="V183" s="1"/>
-    </row>
-    <row r="184" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="W183" s="1"/>
+      <c r="X183" s="1"/>
+    </row>
+    <row r="184" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A184" s="1"/>
       <c r="B184" s="1"/>
       <c r="C184" s="1"/>
@@ -5000,8 +5429,10 @@
       <c r="T184" s="1"/>
       <c r="U184" s="1"/>
       <c r="V184" s="1"/>
-    </row>
-    <row r="185" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="W184" s="1"/>
+      <c r="X184" s="1"/>
+    </row>
+    <row r="185" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A185" s="1"/>
       <c r="B185" s="1"/>
       <c r="C185" s="1"/>
@@ -5024,8 +5455,10 @@
       <c r="T185" s="1"/>
       <c r="U185" s="1"/>
       <c r="V185" s="1"/>
-    </row>
-    <row r="186" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="W185" s="1"/>
+      <c r="X185" s="1"/>
+    </row>
+    <row r="186" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A186" s="1"/>
       <c r="B186" s="1"/>
       <c r="C186" s="1"/>
@@ -5048,8 +5481,10 @@
       <c r="T186" s="1"/>
       <c r="U186" s="1"/>
       <c r="V186" s="1"/>
-    </row>
-    <row r="187" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="W186" s="1"/>
+      <c r="X186" s="1"/>
+    </row>
+    <row r="187" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A187" s="1"/>
       <c r="B187" s="1"/>
       <c r="C187" s="1"/>
@@ -5072,8 +5507,10 @@
       <c r="T187" s="1"/>
       <c r="U187" s="1"/>
       <c r="V187" s="1"/>
-    </row>
-    <row r="188" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="W187" s="1"/>
+      <c r="X187" s="1"/>
+    </row>
+    <row r="188" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A188" s="1"/>
       <c r="B188" s="1"/>
       <c r="C188" s="1"/>
@@ -5096,8 +5533,10 @@
       <c r="T188" s="1"/>
       <c r="U188" s="1"/>
       <c r="V188" s="1"/>
-    </row>
-    <row r="189" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="W188" s="1"/>
+      <c r="X188" s="1"/>
+    </row>
+    <row r="189" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A189" s="1"/>
       <c r="B189" s="1"/>
       <c r="C189" s="1"/>
@@ -5120,8 +5559,10 @@
       <c r="T189" s="1"/>
       <c r="U189" s="1"/>
       <c r="V189" s="1"/>
-    </row>
-    <row r="190" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="W189" s="1"/>
+      <c r="X189" s="1"/>
+    </row>
+    <row r="190" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A190" s="1"/>
       <c r="B190" s="1"/>
       <c r="C190" s="1"/>
@@ -5144,8 +5585,10 @@
       <c r="T190" s="1"/>
       <c r="U190" s="1"/>
       <c r="V190" s="1"/>
-    </row>
-    <row r="191" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="W190" s="1"/>
+      <c r="X190" s="1"/>
+    </row>
+    <row r="191" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A191" s="1"/>
       <c r="B191" s="1"/>
       <c r="C191" s="1"/>
@@ -5168,8 +5611,10 @@
       <c r="T191" s="1"/>
       <c r="U191" s="1"/>
       <c r="V191" s="1"/>
-    </row>
-    <row r="192" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="W191" s="1"/>
+      <c r="X191" s="1"/>
+    </row>
+    <row r="192" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A192" s="1"/>
       <c r="B192" s="1"/>
       <c r="C192" s="1"/>
@@ -5192,8 +5637,10 @@
       <c r="T192" s="1"/>
       <c r="U192" s="1"/>
       <c r="V192" s="1"/>
-    </row>
-    <row r="193" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="W192" s="1"/>
+      <c r="X192" s="1"/>
+    </row>
+    <row r="193" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A193" s="1"/>
       <c r="B193" s="1"/>
       <c r="C193" s="1"/>
@@ -5216,8 +5663,10 @@
       <c r="T193" s="1"/>
       <c r="U193" s="1"/>
       <c r="V193" s="1"/>
-    </row>
-    <row r="194" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="W193" s="1"/>
+      <c r="X193" s="1"/>
+    </row>
+    <row r="194" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A194" s="1"/>
       <c r="B194" s="1"/>
       <c r="C194" s="1"/>
@@ -5240,8 +5689,10 @@
       <c r="T194" s="1"/>
       <c r="U194" s="1"/>
       <c r="V194" s="1"/>
-    </row>
-    <row r="195" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="W194" s="1"/>
+      <c r="X194" s="1"/>
+    </row>
+    <row r="195" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A195" s="1"/>
       <c r="B195" s="1"/>
       <c r="C195" s="1"/>
@@ -5264,8 +5715,10 @@
       <c r="T195" s="1"/>
       <c r="U195" s="1"/>
       <c r="V195" s="1"/>
-    </row>
-    <row r="196" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="W195" s="1"/>
+      <c r="X195" s="1"/>
+    </row>
+    <row r="196" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A196" s="1"/>
       <c r="B196" s="1"/>
       <c r="C196" s="1"/>
@@ -5288,8 +5741,10 @@
       <c r="T196" s="1"/>
       <c r="U196" s="1"/>
       <c r="V196" s="1"/>
-    </row>
-    <row r="197" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="W196" s="1"/>
+      <c r="X196" s="1"/>
+    </row>
+    <row r="197" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A197" s="1"/>
       <c r="B197" s="1"/>
       <c r="C197" s="1"/>
@@ -5312,8 +5767,10 @@
       <c r="T197" s="1"/>
       <c r="U197" s="1"/>
       <c r="V197" s="1"/>
-    </row>
-    <row r="198" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="W197" s="1"/>
+      <c r="X197" s="1"/>
+    </row>
+    <row r="198" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A198" s="1"/>
       <c r="B198" s="1"/>
       <c r="C198" s="1"/>
@@ -5336,8 +5793,10 @@
       <c r="T198" s="1"/>
       <c r="U198" s="1"/>
       <c r="V198" s="1"/>
-    </row>
-    <row r="199" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="W198" s="1"/>
+      <c r="X198" s="1"/>
+    </row>
+    <row r="199" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A199" s="1"/>
       <c r="B199" s="1"/>
       <c r="C199" s="1"/>
@@ -5360,8 +5819,10 @@
       <c r="T199" s="1"/>
       <c r="U199" s="1"/>
       <c r="V199" s="1"/>
-    </row>
-    <row r="200" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="W199" s="1"/>
+      <c r="X199" s="1"/>
+    </row>
+    <row r="200" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A200" s="1"/>
       <c r="B200" s="1"/>
       <c r="C200" s="1"/>
@@ -5384,8 +5845,10 @@
       <c r="T200" s="1"/>
       <c r="U200" s="1"/>
       <c r="V200" s="1"/>
-    </row>
-    <row r="201" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="W200" s="1"/>
+      <c r="X200" s="1"/>
+    </row>
+    <row r="201" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A201" s="1"/>
       <c r="B201" s="1"/>
       <c r="C201" s="1"/>
@@ -5408,8 +5871,10 @@
       <c r="T201" s="1"/>
       <c r="U201" s="1"/>
       <c r="V201" s="1"/>
-    </row>
-    <row r="202" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="W201" s="1"/>
+      <c r="X201" s="1"/>
+    </row>
+    <row r="202" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A202" s="1"/>
       <c r="B202" s="1"/>
       <c r="C202" s="1"/>
@@ -5432,8 +5897,10 @@
       <c r="T202" s="1"/>
       <c r="U202" s="1"/>
       <c r="V202" s="1"/>
-    </row>
-    <row r="203" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="W202" s="1"/>
+      <c r="X202" s="1"/>
+    </row>
+    <row r="203" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A203" s="1"/>
       <c r="B203" s="1"/>
       <c r="C203" s="1"/>
@@ -5456,8 +5923,10 @@
       <c r="T203" s="1"/>
       <c r="U203" s="1"/>
       <c r="V203" s="1"/>
-    </row>
-    <row r="204" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="W203" s="1"/>
+      <c r="X203" s="1"/>
+    </row>
+    <row r="204" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A204" s="1"/>
       <c r="B204" s="1"/>
       <c r="C204" s="1"/>
@@ -5480,8 +5949,10 @@
       <c r="T204" s="1"/>
       <c r="U204" s="1"/>
       <c r="V204" s="1"/>
-    </row>
-    <row r="205" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="W204" s="1"/>
+      <c r="X204" s="1"/>
+    </row>
+    <row r="205" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A205" s="1"/>
       <c r="B205" s="1"/>
       <c r="C205" s="1"/>
@@ -5504,8 +5975,10 @@
       <c r="T205" s="1"/>
       <c r="U205" s="1"/>
       <c r="V205" s="1"/>
-    </row>
-    <row r="206" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="W205" s="1"/>
+      <c r="X205" s="1"/>
+    </row>
+    <row r="206" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A206" s="1"/>
       <c r="B206" s="1"/>
       <c r="C206" s="1"/>
@@ -5528,8 +6001,10 @@
       <c r="T206" s="1"/>
       <c r="U206" s="1"/>
       <c r="V206" s="1"/>
-    </row>
-    <row r="207" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="W206" s="1"/>
+      <c r="X206" s="1"/>
+    </row>
+    <row r="207" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A207" s="1"/>
       <c r="B207" s="1"/>
       <c r="C207" s="1"/>
@@ -5552,8 +6027,10 @@
       <c r="T207" s="1"/>
       <c r="U207" s="1"/>
       <c r="V207" s="1"/>
-    </row>
-    <row r="208" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="W207" s="1"/>
+      <c r="X207" s="1"/>
+    </row>
+    <row r="208" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A208" s="1"/>
       <c r="B208" s="1"/>
       <c r="C208" s="1"/>
@@ -5576,8 +6053,10 @@
       <c r="T208" s="1"/>
       <c r="U208" s="1"/>
       <c r="V208" s="1"/>
-    </row>
-    <row r="209" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="W208" s="1"/>
+      <c r="X208" s="1"/>
+    </row>
+    <row r="209" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A209" s="1"/>
       <c r="B209" s="1"/>
       <c r="C209" s="1"/>
@@ -5600,8 +6079,10 @@
       <c r="T209" s="1"/>
       <c r="U209" s="1"/>
       <c r="V209" s="1"/>
-    </row>
-    <row r="210" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="W209" s="1"/>
+      <c r="X209" s="1"/>
+    </row>
+    <row r="210" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A210" s="1"/>
       <c r="B210" s="1"/>
       <c r="C210" s="1"/>
@@ -5624,8 +6105,10 @@
       <c r="T210" s="1"/>
       <c r="U210" s="1"/>
       <c r="V210" s="1"/>
-    </row>
-    <row r="211" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="W210" s="1"/>
+      <c r="X210" s="1"/>
+    </row>
+    <row r="211" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A211" s="1"/>
       <c r="B211" s="1"/>
       <c r="C211" s="1"/>
@@ -5648,8 +6131,10 @@
       <c r="T211" s="1"/>
       <c r="U211" s="1"/>
       <c r="V211" s="1"/>
-    </row>
-    <row r="212" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="W211" s="1"/>
+      <c r="X211" s="1"/>
+    </row>
+    <row r="212" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A212" s="1"/>
       <c r="B212" s="1"/>
       <c r="C212" s="1"/>
@@ -5672,8 +6157,10 @@
       <c r="T212" s="1"/>
       <c r="U212" s="1"/>
       <c r="V212" s="1"/>
-    </row>
-    <row r="213" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="W212" s="1"/>
+      <c r="X212" s="1"/>
+    </row>
+    <row r="213" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A213" s="1"/>
       <c r="B213" s="1"/>
       <c r="C213" s="1"/>
@@ -5696,8 +6183,10 @@
       <c r="T213" s="1"/>
       <c r="U213" s="1"/>
       <c r="V213" s="1"/>
-    </row>
-    <row r="214" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="W213" s="1"/>
+      <c r="X213" s="1"/>
+    </row>
+    <row r="214" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A214" s="1"/>
       <c r="B214" s="1"/>
       <c r="C214" s="1"/>
@@ -5720,8 +6209,10 @@
       <c r="T214" s="1"/>
       <c r="U214" s="1"/>
       <c r="V214" s="1"/>
-    </row>
-    <row r="215" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="W214" s="1"/>
+      <c r="X214" s="1"/>
+    </row>
+    <row r="215" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A215" s="1"/>
       <c r="B215" s="1"/>
       <c r="C215" s="1"/>
@@ -5744,8 +6235,10 @@
       <c r="T215" s="1"/>
       <c r="U215" s="1"/>
       <c r="V215" s="1"/>
-    </row>
-    <row r="216" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="W215" s="1"/>
+      <c r="X215" s="1"/>
+    </row>
+    <row r="216" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A216" s="1"/>
       <c r="B216" s="1"/>
       <c r="C216" s="1"/>
@@ -5768,8 +6261,10 @@
       <c r="T216" s="1"/>
       <c r="U216" s="1"/>
       <c r="V216" s="1"/>
-    </row>
-    <row r="217" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="W216" s="1"/>
+      <c r="X216" s="1"/>
+    </row>
+    <row r="217" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A217" s="1"/>
       <c r="B217" s="1"/>
       <c r="C217" s="1"/>
@@ -5792,8 +6287,10 @@
       <c r="T217" s="1"/>
       <c r="U217" s="1"/>
       <c r="V217" s="1"/>
-    </row>
-    <row r="218" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="W217" s="1"/>
+      <c r="X217" s="1"/>
+    </row>
+    <row r="218" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A218" s="1"/>
       <c r="B218" s="1"/>
       <c r="C218" s="1"/>
@@ -5816,8 +6313,10 @@
       <c r="T218" s="1"/>
       <c r="U218" s="1"/>
       <c r="V218" s="1"/>
-    </row>
-    <row r="219" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="W218" s="1"/>
+      <c r="X218" s="1"/>
+    </row>
+    <row r="219" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A219" s="1"/>
       <c r="B219" s="1"/>
       <c r="C219" s="1"/>
@@ -5840,8 +6339,10 @@
       <c r="T219" s="1"/>
       <c r="U219" s="1"/>
       <c r="V219" s="1"/>
-    </row>
-    <row r="220" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="W219" s="1"/>
+      <c r="X219" s="1"/>
+    </row>
+    <row r="220" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A220" s="1"/>
       <c r="B220" s="1"/>
       <c r="C220" s="1"/>
@@ -5864,8 +6365,10 @@
       <c r="T220" s="1"/>
       <c r="U220" s="1"/>
       <c r="V220" s="1"/>
-    </row>
-    <row r="221" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="W220" s="1"/>
+      <c r="X220" s="1"/>
+    </row>
+    <row r="221" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A221" s="1"/>
       <c r="B221" s="1"/>
       <c r="C221" s="1"/>
@@ -5888,8 +6391,10 @@
       <c r="T221" s="1"/>
       <c r="U221" s="1"/>
       <c r="V221" s="1"/>
-    </row>
-    <row r="222" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="W221" s="1"/>
+      <c r="X221" s="1"/>
+    </row>
+    <row r="222" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A222" s="1"/>
       <c r="B222" s="1"/>
       <c r="C222" s="1"/>
@@ -5912,8 +6417,10 @@
       <c r="T222" s="1"/>
       <c r="U222" s="1"/>
       <c r="V222" s="1"/>
-    </row>
-    <row r="223" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="W222" s="1"/>
+      <c r="X222" s="1"/>
+    </row>
+    <row r="223" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A223" s="1"/>
       <c r="B223" s="1"/>
       <c r="C223" s="1"/>
@@ -5936,8 +6443,10 @@
       <c r="T223" s="1"/>
       <c r="U223" s="1"/>
       <c r="V223" s="1"/>
-    </row>
-    <row r="224" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="W223" s="1"/>
+      <c r="X223" s="1"/>
+    </row>
+    <row r="224" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A224" s="1"/>
       <c r="B224" s="1"/>
       <c r="C224" s="1"/>
@@ -5960,8 +6469,10 @@
       <c r="T224" s="1"/>
       <c r="U224" s="1"/>
       <c r="V224" s="1"/>
-    </row>
-    <row r="225" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="W224" s="1"/>
+      <c r="X224" s="1"/>
+    </row>
+    <row r="225" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A225" s="1"/>
       <c r="B225" s="1"/>
       <c r="C225" s="1"/>
@@ -5984,8 +6495,10 @@
       <c r="T225" s="1"/>
       <c r="U225" s="1"/>
       <c r="V225" s="1"/>
-    </row>
-    <row r="226" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="W225" s="1"/>
+      <c r="X225" s="1"/>
+    </row>
+    <row r="226" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A226" s="1"/>
       <c r="B226" s="1"/>
       <c r="C226" s="1"/>
@@ -6008,8 +6521,10 @@
       <c r="T226" s="1"/>
       <c r="U226" s="1"/>
       <c r="V226" s="1"/>
-    </row>
-    <row r="227" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="W226" s="1"/>
+      <c r="X226" s="1"/>
+    </row>
+    <row r="227" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A227" s="1"/>
       <c r="B227" s="1"/>
       <c r="C227" s="1"/>
@@ -6032,8 +6547,10 @@
       <c r="T227" s="1"/>
       <c r="U227" s="1"/>
       <c r="V227" s="1"/>
-    </row>
-    <row r="228" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="W227" s="1"/>
+      <c r="X227" s="1"/>
+    </row>
+    <row r="228" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A228" s="1"/>
       <c r="B228" s="1"/>
       <c r="C228" s="1"/>
@@ -6056,8 +6573,10 @@
       <c r="T228" s="1"/>
       <c r="U228" s="1"/>
       <c r="V228" s="1"/>
-    </row>
-    <row r="229" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="W228" s="1"/>
+      <c r="X228" s="1"/>
+    </row>
+    <row r="229" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A229" s="1"/>
       <c r="B229" s="1"/>
       <c r="C229" s="1"/>
@@ -6080,8 +6599,10 @@
       <c r="T229" s="1"/>
       <c r="U229" s="1"/>
       <c r="V229" s="1"/>
-    </row>
-    <row r="230" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="W229" s="1"/>
+      <c r="X229" s="1"/>
+    </row>
+    <row r="230" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A230" s="1"/>
       <c r="B230" s="1"/>
       <c r="C230" s="1"/>
@@ -6104,8 +6625,10 @@
       <c r="T230" s="1"/>
       <c r="U230" s="1"/>
       <c r="V230" s="1"/>
-    </row>
-    <row r="231" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="W230" s="1"/>
+      <c r="X230" s="1"/>
+    </row>
+    <row r="231" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A231" s="1"/>
       <c r="B231" s="1"/>
       <c r="C231" s="1"/>
@@ -6128,8 +6651,10 @@
       <c r="T231" s="1"/>
       <c r="U231" s="1"/>
       <c r="V231" s="1"/>
-    </row>
-    <row r="232" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="W231" s="1"/>
+      <c r="X231" s="1"/>
+    </row>
+    <row r="232" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A232" s="1"/>
       <c r="B232" s="1"/>
       <c r="C232" s="1"/>
@@ -6152,8 +6677,10 @@
       <c r="T232" s="1"/>
       <c r="U232" s="1"/>
       <c r="V232" s="1"/>
-    </row>
-    <row r="233" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="W232" s="1"/>
+      <c r="X232" s="1"/>
+    </row>
+    <row r="233" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A233" s="1"/>
       <c r="B233" s="1"/>
       <c r="C233" s="1"/>
@@ -6176,8 +6703,10 @@
       <c r="T233" s="1"/>
       <c r="U233" s="1"/>
       <c r="V233" s="1"/>
-    </row>
-    <row r="234" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="W233" s="1"/>
+      <c r="X233" s="1"/>
+    </row>
+    <row r="234" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A234" s="1"/>
       <c r="B234" s="1"/>
       <c r="C234" s="1"/>
@@ -6200,8 +6729,10 @@
       <c r="T234" s="1"/>
       <c r="U234" s="1"/>
       <c r="V234" s="1"/>
-    </row>
-    <row r="235" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="W234" s="1"/>
+      <c r="X234" s="1"/>
+    </row>
+    <row r="235" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A235" s="1"/>
       <c r="B235" s="1"/>
       <c r="C235" s="1"/>
@@ -6224,8 +6755,10 @@
       <c r="T235" s="1"/>
       <c r="U235" s="1"/>
       <c r="V235" s="1"/>
-    </row>
-    <row r="236" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="W235" s="1"/>
+      <c r="X235" s="1"/>
+    </row>
+    <row r="236" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A236" s="1"/>
       <c r="B236" s="1"/>
       <c r="C236" s="1"/>
@@ -6248,8 +6781,10 @@
       <c r="T236" s="1"/>
       <c r="U236" s="1"/>
       <c r="V236" s="1"/>
-    </row>
-    <row r="237" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="W236" s="1"/>
+      <c r="X236" s="1"/>
+    </row>
+    <row r="237" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A237" s="1"/>
       <c r="B237" s="1"/>
       <c r="C237" s="1"/>
@@ -6272,8 +6807,10 @@
       <c r="T237" s="1"/>
       <c r="U237" s="1"/>
       <c r="V237" s="1"/>
-    </row>
-    <row r="238" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="W237" s="1"/>
+      <c r="X237" s="1"/>
+    </row>
+    <row r="238" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A238" s="1"/>
       <c r="B238" s="1"/>
       <c r="C238" s="1"/>
@@ -6296,8 +6833,10 @@
       <c r="T238" s="1"/>
       <c r="U238" s="1"/>
       <c r="V238" s="1"/>
-    </row>
-    <row r="239" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="W238" s="1"/>
+      <c r="X238" s="1"/>
+    </row>
+    <row r="239" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A239" s="1"/>
       <c r="B239" s="1"/>
       <c r="C239" s="1"/>
@@ -6320,8 +6859,10 @@
       <c r="T239" s="1"/>
       <c r="U239" s="1"/>
       <c r="V239" s="1"/>
-    </row>
-    <row r="240" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="W239" s="1"/>
+      <c r="X239" s="1"/>
+    </row>
+    <row r="240" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A240" s="1"/>
       <c r="B240" s="1"/>
       <c r="C240" s="1"/>
@@ -6344,8 +6885,10 @@
       <c r="T240" s="1"/>
       <c r="U240" s="1"/>
       <c r="V240" s="1"/>
-    </row>
-    <row r="241" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="W240" s="1"/>
+      <c r="X240" s="1"/>
+    </row>
+    <row r="241" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A241" s="1"/>
       <c r="B241" s="1"/>
       <c r="C241" s="1"/>
@@ -6368,8 +6911,10 @@
       <c r="T241" s="1"/>
       <c r="U241" s="1"/>
       <c r="V241" s="1"/>
-    </row>
-    <row r="242" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="W241" s="1"/>
+      <c r="X241" s="1"/>
+    </row>
+    <row r="242" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A242" s="1"/>
       <c r="B242" s="1"/>
       <c r="C242" s="1"/>
@@ -6392,8 +6937,10 @@
       <c r="T242" s="1"/>
       <c r="U242" s="1"/>
       <c r="V242" s="1"/>
-    </row>
-    <row r="243" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="W242" s="1"/>
+      <c r="X242" s="1"/>
+    </row>
+    <row r="243" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A243" s="1"/>
       <c r="B243" s="1"/>
       <c r="C243" s="1"/>
@@ -6416,8 +6963,10 @@
       <c r="T243" s="1"/>
       <c r="U243" s="1"/>
       <c r="V243" s="1"/>
-    </row>
-    <row r="244" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="W243" s="1"/>
+      <c r="X243" s="1"/>
+    </row>
+    <row r="244" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A244" s="1"/>
       <c r="B244" s="1"/>
       <c r="C244" s="1"/>
@@ -6440,8 +6989,10 @@
       <c r="T244" s="1"/>
       <c r="U244" s="1"/>
       <c r="V244" s="1"/>
-    </row>
-    <row r="245" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="W244" s="1"/>
+      <c r="X244" s="1"/>
+    </row>
+    <row r="245" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A245" s="1"/>
       <c r="B245" s="1"/>
       <c r="C245" s="1"/>
@@ -6464,8 +7015,10 @@
       <c r="T245" s="1"/>
       <c r="U245" s="1"/>
       <c r="V245" s="1"/>
-    </row>
-    <row r="246" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="W245" s="1"/>
+      <c r="X245" s="1"/>
+    </row>
+    <row r="246" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A246" s="1"/>
       <c r="B246" s="1"/>
       <c r="C246" s="1"/>
@@ -6488,8 +7041,10 @@
       <c r="T246" s="1"/>
       <c r="U246" s="1"/>
       <c r="V246" s="1"/>
-    </row>
-    <row r="247" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="W246" s="1"/>
+      <c r="X246" s="1"/>
+    </row>
+    <row r="247" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A247" s="1"/>
       <c r="B247" s="1"/>
       <c r="C247" s="1"/>
@@ -6512,8 +7067,10 @@
       <c r="T247" s="1"/>
       <c r="U247" s="1"/>
       <c r="V247" s="1"/>
-    </row>
-    <row r="248" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="W247" s="1"/>
+      <c r="X247" s="1"/>
+    </row>
+    <row r="248" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A248" s="1"/>
       <c r="B248" s="1"/>
       <c r="C248" s="1"/>
@@ -6536,8 +7093,10 @@
       <c r="T248" s="1"/>
       <c r="U248" s="1"/>
       <c r="V248" s="1"/>
-    </row>
-    <row r="249" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="W248" s="1"/>
+      <c r="X248" s="1"/>
+    </row>
+    <row r="249" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A249" s="1"/>
       <c r="B249" s="1"/>
       <c r="C249" s="1"/>
@@ -6560,8 +7119,10 @@
       <c r="T249" s="1"/>
       <c r="U249" s="1"/>
       <c r="V249" s="1"/>
-    </row>
-    <row r="250" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="W249" s="1"/>
+      <c r="X249" s="1"/>
+    </row>
+    <row r="250" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A250" s="1"/>
       <c r="B250" s="1"/>
       <c r="C250" s="1"/>
@@ -6584,8 +7145,10 @@
       <c r="T250" s="1"/>
       <c r="U250" s="1"/>
       <c r="V250" s="1"/>
-    </row>
-    <row r="251" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="W250" s="1"/>
+      <c r="X250" s="1"/>
+    </row>
+    <row r="251" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A251" s="1"/>
       <c r="B251" s="1"/>
       <c r="C251" s="1"/>
@@ -6608,8 +7171,10 @@
       <c r="T251" s="1"/>
       <c r="U251" s="1"/>
       <c r="V251" s="1"/>
-    </row>
-    <row r="252" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="W251" s="1"/>
+      <c r="X251" s="1"/>
+    </row>
+    <row r="252" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A252" s="1"/>
       <c r="B252" s="1"/>
       <c r="C252" s="1"/>
@@ -6632,8 +7197,10 @@
       <c r="T252" s="1"/>
       <c r="U252" s="1"/>
       <c r="V252" s="1"/>
-    </row>
-    <row r="253" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="W252" s="1"/>
+      <c r="X252" s="1"/>
+    </row>
+    <row r="253" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A253" s="1"/>
       <c r="B253" s="1"/>
       <c r="C253" s="1"/>
@@ -6656,8 +7223,10 @@
       <c r="T253" s="1"/>
       <c r="U253" s="1"/>
       <c r="V253" s="1"/>
-    </row>
-    <row r="254" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="W253" s="1"/>
+      <c r="X253" s="1"/>
+    </row>
+    <row r="254" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A254" s="1"/>
       <c r="B254" s="1"/>
       <c r="C254" s="1"/>
@@ -6680,8 +7249,10 @@
       <c r="T254" s="1"/>
       <c r="U254" s="1"/>
       <c r="V254" s="1"/>
-    </row>
-    <row r="255" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="W254" s="1"/>
+      <c r="X254" s="1"/>
+    </row>
+    <row r="255" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A255" s="1"/>
       <c r="B255" s="1"/>
       <c r="C255" s="1"/>
@@ -6704,8 +7275,10 @@
       <c r="T255" s="1"/>
       <c r="U255" s="1"/>
       <c r="V255" s="1"/>
-    </row>
-    <row r="256" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="W255" s="1"/>
+      <c r="X255" s="1"/>
+    </row>
+    <row r="256" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A256" s="1"/>
       <c r="B256" s="1"/>
       <c r="C256" s="1"/>
@@ -6728,6 +7301,8 @@
       <c r="T256" s="1"/>
       <c r="U256" s="1"/>
       <c r="V256" s="1"/>
+      <c r="W256" s="1"/>
+      <c r="X256" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>